<commit_message>
menyelesakian bayar beli car premi reguler positive
</commit_message>
<xml_diff>
--- a/Bayar Beli - CAR Tagihan Lainnya/Default.xlsx
+++ b/Bayar Beli - CAR Tagihan Lainnya/Default.xlsx
@@ -14,41 +14,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
-  <si>
-    <t>PROJECT_NAME</t>
-  </si>
-  <si>
-    <t>SuperApps-BSI Super Apps versi 1.0.2 (7761)</t>
-  </si>
-  <si>
-    <t>COMPANY_LOGO</t>
-  </si>
-  <si>
-    <t>SCREEN_SHOOT</t>
-  </si>
-  <si>
-    <t>COVER_TITLE</t>
-  </si>
-  <si>
-    <t>D:\Mentahan\PlugIn UFT\Napalm\Napalm\libray\BSILOGO.jpeg</t>
-  </si>
-  <si>
-    <t>SuperApps-BSIMobile</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>COVER_SUBTITLE</t>
-  </si>
-  <si>
-    <t>Automation Testing - SuperApps-BSIMobile</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -189,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -197,43 +162,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -532,59 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="1" width="10.75390625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.48828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.37109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.3671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -600,10 +492,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>